<commit_message>
recent posts and updates
</commit_message>
<xml_diff>
--- a/static/csv/pubs.xlsx
+++ b/static/csv/pubs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\scagg\Documents\Shane's Projects\folio\static\csv\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C793DFD9-535E-414F-9142-9AF31EDAFF57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77712CD1-0EB2-42FA-BF2A-06E14B1FA9E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15525" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15525" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="citations" sheetId="1" r:id="rId1"/>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="39">
   <si>
     <t>Year</t>
   </si>
@@ -168,19 +168,10 @@
     <t>2022Piperata</t>
   </si>
   <si>
-    <t>(submitted)</t>
-  </si>
-  <si>
     <t>(in review)</t>
   </si>
   <si>
     <t xml:space="preserve">Piperata, B., Scaggs, S., Dufour, D., Adams, I. (in review) Measuring food security: An introduction to tools for human biologists and ecologists. American Journal of Human Biology. </t>
-  </si>
-  <si>
-    <t>2022Downey</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Downey,S., Moschler, J., Penados, F., Peterman, W., Qin, R., Scaggs, S., Shuang, S., Walker, M. (submitted). Indigenous Maya swidden practices increase tropical biodiversity in community forests. Proceedings of the National Academy of Sciences. </t>
   </si>
 </sst>
 </file>
@@ -1024,10 +1015,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1052,12 +1043,12 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>2022</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C2" t="s">
         <v>37</v>
@@ -1066,24 +1057,24 @@
         <v>35</v>
       </c>
       <c r="E2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>2022</v>
+        <v>2021</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>39</v>
+        <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>38</v>
+        <v>5</v>
       </c>
       <c r="D3" t="s">
-        <v>35</v>
+        <v>6</v>
       </c>
       <c r="E3" t="s">
-        <v>36</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -1091,33 +1082,33 @@
         <v>2021</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C4" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D4" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="E4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>2021</v>
+        <v>2020</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C5" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="D5" t="s">
         <v>9</v>
       </c>
       <c r="E5" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -1125,66 +1116,49 @@
         <v>2020</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C6" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D6" t="s">
         <v>9</v>
       </c>
       <c r="E6" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>2020</v>
+        <v>2019</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C7" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D7" t="s">
         <v>9</v>
       </c>
       <c r="E7" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>2019</v>
+        <v>2017</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C8" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D8" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="E8" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>2017</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C9" t="s">
-        <v>17</v>
-      </c>
-      <c r="D9" t="s">
-        <v>18</v>
-      </c>
-      <c r="E9" t="s">
         <v>26</v>
       </c>
     </row>
@@ -1195,66 +1169,62 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:I9"/>
+  <dimension ref="A1:H9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="29.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B1" s="1" t="str" cm="1">
-        <f t="array" ref="B1:I1">TRANSPOSE(citations!E2:E9)</f>
-        <v>2022Downey</v>
+        <f t="array" ref="B1:H1">TRANSPOSE(citations!E2:E8)</f>
+        <v>2022Piperata</v>
       </c>
       <c r="C1" s="1" t="str">
-        <v>2022Piperata</v>
+        <v>2021Scaggs</v>
       </c>
       <c r="D1" s="1" t="str">
-        <v>2021Scaggs</v>
+        <v>2021Kawa</v>
       </c>
       <c r="E1" s="1" t="str">
-        <v>2021Kawa</v>
+        <v>2020Downey</v>
       </c>
       <c r="F1" s="1" t="str">
-        <v>2020Downey</v>
+        <v>2020Moritz</v>
       </c>
       <c r="G1" s="1" t="str">
-        <v>2020Moritz</v>
+        <v>2019Snopkowski</v>
       </c>
       <c r="H1" s="1" t="str">
-        <v>2019Snopkowski</v>
-      </c>
-      <c r="I1" s="1" t="str">
         <v>2017Scaggs</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>27</v>
       </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
       <c r="C2">
         <v>1</v>
       </c>
-      <c r="D2">
+      <c r="G2">
         <v>1</v>
       </c>
       <c r="H2">
         <v>1</v>
       </c>
-      <c r="I2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>28</v>
       </c>
@@ -1264,27 +1234,24 @@
       <c r="C3">
         <v>1</v>
       </c>
-      <c r="D3">
+      <c r="E3">
         <v>1</v>
       </c>
       <c r="F3">
         <v>1</v>
       </c>
-      <c r="G3">
-        <v>1</v>
-      </c>
-      <c r="I3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>29</v>
       </c>
       <c r="B4">
         <v>1</v>
       </c>
-      <c r="C4">
+      <c r="E4">
         <v>1</v>
       </c>
       <c r="F4">
@@ -1296,24 +1263,21 @@
       <c r="H4">
         <v>1</v>
       </c>
-      <c r="I4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>30</v>
       </c>
-      <c r="I5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>32</v>
       </c>
@@ -1323,7 +1287,7 @@
       <c r="C7">
         <v>1</v>
       </c>
-      <c r="D7">
+      <c r="E7">
         <v>1</v>
       </c>
       <c r="F7">
@@ -1335,11 +1299,8 @@
       <c r="H7">
         <v>1</v>
       </c>
-      <c r="I7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>33</v>
       </c>
@@ -1364,15 +1325,12 @@
       <c r="H8">
         <v>1</v>
       </c>
-      <c r="I8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>34</v>
       </c>
-      <c r="D9">
+      <c r="C9">
         <v>1</v>
       </c>
     </row>

</xml_diff>